<commit_message>
Added documentation, video and code optimizations.
</commit_message>
<xml_diff>
--- a/Aspose.Assignment/Aspose.Web/Samples/Employees.xlsx
+++ b/Aspose.Assignment/Aspose.Web/Samples/Employees.xlsx
@@ -4,107 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="615" windowWidth="22695" windowHeight="15780"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="14385"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
-  <si>
-    <t>Ann Chavez</t>
-  </si>
-  <si>
-    <t>achavez0@wikispaces.com</t>
-  </si>
-  <si>
-    <t>Craig Russell</t>
-  </si>
-  <si>
-    <t>crussell1@cnbc.com</t>
-  </si>
-  <si>
-    <t>Carlos Bennett</t>
-  </si>
-  <si>
-    <t>cbennett2@myspace.com</t>
-  </si>
-  <si>
-    <t>Benjamin Watkins</t>
-  </si>
-  <si>
-    <t>bwatkins3@geocities.jp</t>
-  </si>
-  <si>
-    <t>Janice Hayes</t>
-  </si>
-  <si>
-    <t>jhayes4@youtu.be</t>
-  </si>
-  <si>
-    <t>Jimmy Wright</t>
-  </si>
-  <si>
-    <t>jwright5@utexas.edu</t>
-  </si>
-  <si>
-    <t>Nancy Walker</t>
-  </si>
-  <si>
-    <t>nwalker6@cnbc.com</t>
-  </si>
-  <si>
-    <t>Rachel Hicks</t>
-  </si>
-  <si>
-    <t>rhicks7@mac.com</t>
-  </si>
-  <si>
-    <t>Cynthia Chapman</t>
-  </si>
-  <si>
-    <t>cchapman8@nature.com</t>
-  </si>
-  <si>
-    <t>Anthony Thompson</t>
-  </si>
-  <si>
-    <t>athompson9@oaic.gov.au</t>
-  </si>
-  <si>
-    <t>027 Oriole Park , Vista Hermosa</t>
-  </si>
-  <si>
-    <t>00440 Kim Center , Torre</t>
-  </si>
-  <si>
-    <t>9637 Westend Trail , Gomunice</t>
-  </si>
-  <si>
-    <t>59 Stone Corner Hill , Al Jubayhah</t>
-  </si>
-  <si>
-    <t>37 Ramsey Parkway , Mamuša</t>
-  </si>
-  <si>
-    <t>93760 Del Mar Avenue , Cassanayan</t>
-  </si>
-  <si>
-    <t>204 Ruskin Parkway , Swellendam</t>
-  </si>
-  <si>
-    <t>35 Lakewood Trail , Niihama</t>
-  </si>
-  <si>
-    <t>53988 Morrow Drive , Washington</t>
-  </si>
-  <si>
-    <t>7690 Kingsford Park , Chuchkovo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Address</t>
   </si>
@@ -112,21 +24,40 @@
     <t>Salary</t>
   </si>
   <si>
+    <t>Maria Shahid</t>
+  </si>
+  <si>
+    <t>A-57, Block 1, Gulshan-e-Iqbal, Karachi</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>FullName</t>
+    <t>maria.shahid112@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
-      <family val="1"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,17 +77,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -452,175 +387,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.125" customWidth="1"/>
-    <col min="4" max="4" width="10.75" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>64917.19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3">
-        <v>58341.88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4">
-        <v>88015.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5">
-        <v>67203.320000000007</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6">
-        <v>54417.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7">
-        <v>89861.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8">
-        <v>78915.66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9">
-        <v>53073.77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10">
-        <v>85795.57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11">
-        <v>97289.68</v>
+      <c r="D2" s="2">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>